<commit_message>
Condensamento dos crimes/Criação do índice mensal de criminalidade
</commit_message>
<xml_diff>
--- a/Dados_penas.xlsx
+++ b/Dados_penas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\persp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Trabalhos de Programação\Crimes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A31259E0-FADF-4265-8176-81CF2C91C10B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9473397-A119-4010-9A31-3E70E9AB59E7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4920" xr2:uid="{EF2FEF4C-8FCF-4514-8B5D-816260BF5F45}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Crime</t>
   </si>
@@ -51,51 +51,6 @@
     <t>Lesão Corporal Culposa</t>
   </si>
   <si>
-    <t>Roubo a Comércio</t>
-  </si>
-  <si>
-    <t>Roubo a Residência</t>
-  </si>
-  <si>
-    <t>Roubo de Veículo</t>
-  </si>
-  <si>
-    <t>Roubo de Carga</t>
-  </si>
-  <si>
-    <t>Roubo a Transeunte</t>
-  </si>
-  <si>
-    <t>Roubo em Coletivo</t>
-  </si>
-  <si>
-    <t>Roubo a Banco</t>
-  </si>
-  <si>
-    <t>Roubo a Caixa Eletrônico</t>
-  </si>
-  <si>
-    <t>Roubo de Celular</t>
-  </si>
-  <si>
-    <t>Roubo com Condução para Saque</t>
-  </si>
-  <si>
-    <t>Roubo a Bicicleta</t>
-  </si>
-  <si>
-    <t>Outros Roubos</t>
-  </si>
-  <si>
-    <t>Furto de Veículos</t>
-  </si>
-  <si>
-    <t>Furto de Bicicleta</t>
-  </si>
-  <si>
-    <t>Outros Furtos</t>
-  </si>
-  <si>
     <t>Sequestro</t>
   </si>
   <si>
@@ -118,6 +73,12 @@
   </si>
   <si>
     <t>Pena mínima</t>
+  </si>
+  <si>
+    <t>Roubos</t>
+  </si>
+  <si>
+    <t>Furtos</t>
   </si>
 </sst>
 </file>
@@ -493,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769843BB-23C6-4EC8-A9D1-30BD8978D1F0}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,10 +472,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -575,7 +536,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -608,7 +569,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1">
         <v>4</v>
@@ -619,210 +580,67 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
         <v>4</v>
-      </c>
-      <c r="C11" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2">
         <v>12</v>
-      </c>
-      <c r="B14" s="1">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2">
-        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C16" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1">
-        <v>4</v>
-      </c>
-      <c r="C17" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1">
-        <v>4</v>
-      </c>
-      <c r="C18" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1">
-        <v>4</v>
-      </c>
-      <c r="C19" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1">
-        <v>4</v>
-      </c>
-      <c r="C20" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1">
-        <v>4</v>
-      </c>
-      <c r="C21" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1">
-        <v>8</v>
-      </c>
-      <c r="C26" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="1">
-        <v>6</v>
-      </c>
-      <c r="C27" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="4">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C29" s="2">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>